<commit_message>
merging external data files with ecoregions
</commit_message>
<xml_diff>
--- a/Benchmarks/Water Chemistry/External Data/NRSA_WQ.xlsx
+++ b/Benchmarks/Water Chemistry/External Data/NRSA_WQ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateoforegon-my.sharepoint.com/personal/adam_thompson_deq_oregon_gov/Documents/Documents/BioMonORDEQ/Benchmarks/Water Chemistry/External Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateoforegon-my.sharepoint.com/personal/sabine_berzins_deq_oregon_gov/Documents/Documents/BioMonORDEQ/Benchmarks/Water Chemistry/External Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="362" documentId="8_{20EC14D1-7659-476B-B0D0-76EEE484300F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45B88F46-ACC6-4D88-8406-F5F41345F0A7}"/>
+  <xr:revisionPtr revIDLastSave="370" documentId="8_{20EC14D1-7659-476B-B0D0-76EEE484300F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE342462-7ACB-4851-B477-37E96CB08901}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="1040" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$IF$184</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15036" uniqueCount="1441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15402" uniqueCount="1452">
   <si>
     <t>UID</t>
   </si>
@@ -4361,13 +4361,46 @@
   </si>
   <si>
     <t>Boatable or Wadeable</t>
+  </si>
+  <si>
+    <t>Columbia Plateau</t>
+  </si>
+  <si>
+    <t>COLD DESERTS</t>
+  </si>
+  <si>
+    <t>Blue Mountains</t>
+  </si>
+  <si>
+    <t>WESTERN CORDILLERA</t>
+  </si>
+  <si>
+    <t>Coast Range</t>
+  </si>
+  <si>
+    <t>MARINE WEST COAST FOREST</t>
+  </si>
+  <si>
+    <t>Willamette Valley</t>
+  </si>
+  <si>
+    <t>Cascades</t>
+  </si>
+  <si>
+    <t>Eastern Cascades Slopes and Foothills</t>
+  </si>
+  <si>
+    <t>Northern Basin and Range</t>
+  </si>
+  <si>
+    <t>Klamath Mountains</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4390,6 +4423,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -4468,8 +4506,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4601,8 +4640,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{4E99AF99-C912-440D-99E6-613492AA28AD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -62542,10 +62582,10 @@
   <dimension ref="A1:AU184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F134" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="H141" sqref="H141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -62615,10 +62655,10 @@
         <v>1436</v>
       </c>
       <c r="H1" s="38" t="s">
+        <v>1438</v>
+      </c>
+      <c r="I1" s="38" t="s">
         <v>1437</v>
-      </c>
-      <c r="I1" s="38" t="s">
-        <v>1438</v>
       </c>
       <c r="J1" s="38" t="s">
         <v>1439</v>
@@ -62757,6 +62797,12 @@
       <c r="G2">
         <v>23685528</v>
       </c>
+      <c r="H2" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1442</v>
+      </c>
       <c r="K2" s="56"/>
       <c r="L2" s="30">
         <v>7.0000000000000001E-3</v>
@@ -62889,6 +62935,12 @@
       <c r="G3">
         <v>23686016</v>
       </c>
+      <c r="H3" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1444</v>
+      </c>
       <c r="K3" s="56"/>
       <c r="L3" s="30">
         <v>8.0000000000000002E-3</v>
@@ -63021,6 +63073,12 @@
       <c r="G4">
         <v>23442327</v>
       </c>
+      <c r="H4" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1444</v>
+      </c>
       <c r="K4" s="56"/>
       <c r="L4" s="30">
         <v>4.0000000000000001E-3</v>
@@ -63153,6 +63211,12 @@
       <c r="G5">
         <v>23875969</v>
       </c>
+      <c r="H5" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1446</v>
+      </c>
       <c r="K5" s="56"/>
       <c r="L5" s="29">
         <v>5.0000000000000001E-4</v>
@@ -63285,6 +63349,12 @@
       <c r="G6">
         <v>23442327</v>
       </c>
+      <c r="H6" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1444</v>
+      </c>
       <c r="K6" s="56"/>
       <c r="L6" s="30">
         <v>8.9999999999999993E-3</v>
@@ -63417,6 +63487,12 @@
       <c r="G7">
         <v>23875969</v>
       </c>
+      <c r="H7" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1446</v>
+      </c>
       <c r="K7" s="56"/>
       <c r="L7" s="30">
         <v>1.4999999999999999E-2</v>
@@ -63549,6 +63625,12 @@
       <c r="G8">
         <v>23804876</v>
       </c>
+      <c r="H8" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1446</v>
+      </c>
       <c r="K8" s="56"/>
       <c r="L8" s="30">
         <v>0.04</v>
@@ -63681,6 +63763,12 @@
       <c r="G9">
         <v>23428648</v>
       </c>
+      <c r="H9" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1444</v>
+      </c>
       <c r="K9" s="56"/>
       <c r="L9" s="30">
         <v>0.01</v>
@@ -63813,6 +63901,12 @@
       <c r="G10">
         <v>23671143</v>
       </c>
+      <c r="H10" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1444</v>
+      </c>
       <c r="K10" s="56"/>
       <c r="L10" s="30">
         <v>4.0000000000000001E-3</v>
@@ -63945,6 +64039,12 @@
       <c r="G11">
         <v>24208825</v>
       </c>
+      <c r="H11" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1444</v>
+      </c>
       <c r="K11" s="56"/>
       <c r="L11" s="30">
         <v>4.0000000000000001E-3</v>
@@ -64077,6 +64177,12 @@
       <c r="G12">
         <v>23785691</v>
       </c>
+      <c r="H12" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1446</v>
+      </c>
       <c r="K12" s="56"/>
       <c r="L12" s="30">
         <v>7.0000000000000001E-3</v>
@@ -64209,6 +64315,12 @@
       <c r="G13">
         <v>23773217</v>
       </c>
+      <c r="H13" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1444</v>
+      </c>
       <c r="K13" s="56"/>
       <c r="L13" s="30">
         <v>3.0000000000000001E-3</v>
@@ -64341,6 +64453,12 @@
       <c r="G14" s="52">
         <v>23753122</v>
       </c>
+      <c r="H14" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1444</v>
+      </c>
       <c r="K14" s="56"/>
       <c r="L14" s="30">
         <v>4.0000000000000001E-3</v>
@@ -64473,6 +64591,12 @@
       <c r="G15" s="52">
         <v>23780817</v>
       </c>
+      <c r="H15" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1444</v>
+      </c>
       <c r="K15" s="56"/>
       <c r="L15" s="30">
         <v>4.0000000000000001E-3</v>
@@ -64605,6 +64729,12 @@
       <c r="G16">
         <v>23781157</v>
       </c>
+      <c r="H16" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1444</v>
+      </c>
       <c r="K16" s="56"/>
       <c r="L16" s="30">
         <v>4.0000000000000001E-3</v>
@@ -64737,6 +64867,12 @@
       <c r="G17">
         <v>23785691</v>
       </c>
+      <c r="H17" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1446</v>
+      </c>
       <c r="K17" s="56"/>
       <c r="L17" s="30">
         <v>8.0000000000000002E-3</v>
@@ -64869,6 +65005,12 @@
       <c r="G18" s="52">
         <v>23719577</v>
       </c>
+      <c r="H18" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1444</v>
+      </c>
       <c r="K18" s="56"/>
       <c r="L18" s="30">
         <v>1.6E-2</v>
@@ -65001,6 +65143,12 @@
       <c r="G19" s="52">
         <v>23718769</v>
       </c>
+      <c r="H19" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1442</v>
+      </c>
       <c r="K19" s="56"/>
       <c r="L19" s="30">
         <v>1.2E-2</v>
@@ -65133,6 +65281,12 @@
       <c r="G20">
         <v>23914479</v>
       </c>
+      <c r="H20" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I20" t="s">
+        <v>1446</v>
+      </c>
       <c r="K20" s="56"/>
       <c r="L20" s="30">
         <v>6.0000000000000001E-3</v>
@@ -65265,6 +65419,12 @@
       <c r="G21">
         <v>23915243</v>
       </c>
+      <c r="H21" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I21" t="s">
+        <v>1446</v>
+      </c>
       <c r="K21" s="56"/>
       <c r="L21" s="30">
         <v>6.0000000000000001E-3</v>
@@ -65397,6 +65557,12 @@
       <c r="G22">
         <v>23940179</v>
       </c>
+      <c r="H22" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1446</v>
+      </c>
       <c r="K22" s="56"/>
       <c r="L22" s="30">
         <v>2.1000000000000001E-2</v>
@@ -65529,6 +65695,12 @@
       <c r="G23">
         <v>23902339</v>
       </c>
+      <c r="H23" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1444</v>
+      </c>
       <c r="K23" s="56"/>
       <c r="L23" s="30">
         <v>3.0000000000000001E-3</v>
@@ -65661,6 +65833,12 @@
       <c r="G24">
         <v>24084650</v>
       </c>
+      <c r="H24" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1444</v>
+      </c>
       <c r="K24" s="56"/>
       <c r="L24" s="30">
         <v>4.0000000000000001E-3</v>
@@ -65793,6 +65971,12 @@
       <c r="G25">
         <v>24084412</v>
       </c>
+      <c r="H25" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I25" t="s">
+        <v>1444</v>
+      </c>
       <c r="K25" s="56"/>
       <c r="L25" s="30">
         <v>8.0000000000000002E-3</v>
@@ -65925,6 +66109,12 @@
       <c r="G26">
         <v>24013601</v>
       </c>
+      <c r="H26" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1442</v>
+      </c>
       <c r="K26" s="56"/>
       <c r="L26" s="30">
         <v>7.0000000000000001E-3</v>
@@ -66057,6 +66247,12 @@
       <c r="G27">
         <v>24013655</v>
       </c>
+      <c r="H27" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1442</v>
+      </c>
       <c r="K27" s="56"/>
       <c r="L27" s="30">
         <v>1.0999999999999999E-2</v>
@@ -66189,6 +66385,12 @@
       <c r="G28">
         <v>23886302</v>
       </c>
+      <c r="H28" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I28" t="s">
+        <v>1446</v>
+      </c>
       <c r="K28" s="56"/>
       <c r="L28" s="30">
         <v>1.4E-2</v>
@@ -66321,6 +66523,12 @@
       <c r="G29">
         <v>24526788</v>
       </c>
+      <c r="H29" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1446</v>
+      </c>
       <c r="K29" s="56"/>
       <c r="L29" s="30">
         <v>3.0000000000000001E-3</v>
@@ -66453,6 +66661,12 @@
       <c r="G30">
         <v>23889554</v>
       </c>
+      <c r="H30" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1446</v>
+      </c>
       <c r="K30" s="56"/>
       <c r="L30" s="30">
         <v>8.9999999999999993E-3</v>
@@ -66585,6 +66799,12 @@
       <c r="G31">
         <v>24143358</v>
       </c>
+      <c r="H31" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1442</v>
+      </c>
       <c r="K31" s="56"/>
       <c r="L31" s="30">
         <v>5.0000000000000001E-3</v>
@@ -66717,6 +66937,12 @@
       <c r="G32">
         <v>24544171</v>
       </c>
+      <c r="H32" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1442</v>
+      </c>
       <c r="K32" s="56"/>
       <c r="L32" s="30">
         <v>1.4999999999999999E-2</v>
@@ -66849,6 +67075,12 @@
       <c r="G33">
         <v>23685656</v>
       </c>
+      <c r="H33" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1442</v>
+      </c>
       <c r="K33" s="56"/>
       <c r="L33" s="30">
         <v>8.9999999999999993E-3</v>
@@ -66981,6 +67213,12 @@
       <c r="G34">
         <v>23659414</v>
       </c>
+      <c r="H34" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1442</v>
+      </c>
       <c r="K34" s="56"/>
       <c r="L34" s="30">
         <v>8.6999999999999994E-2</v>
@@ -67113,6 +67351,12 @@
       <c r="G35">
         <v>23686254</v>
       </c>
+      <c r="H35" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1444</v>
+      </c>
       <c r="K35" s="56"/>
       <c r="L35" s="30">
         <v>1.2E-2</v>
@@ -67245,6 +67489,12 @@
       <c r="G36">
         <v>23700195</v>
       </c>
+      <c r="H36" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I36" t="s">
+        <v>1444</v>
+      </c>
       <c r="K36" s="56"/>
       <c r="L36" s="30">
         <v>5.0000000000000001E-3</v>
@@ -67377,6 +67627,12 @@
       <c r="G37">
         <v>23713968</v>
       </c>
+      <c r="H37" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I37" t="s">
+        <v>1444</v>
+      </c>
       <c r="K37" s="56"/>
       <c r="L37" s="30">
         <v>8.9999999999999993E-3</v>
@@ -67509,6 +67765,12 @@
       <c r="G38">
         <v>23760158</v>
       </c>
+      <c r="H38" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I38" t="s">
+        <v>1444</v>
+      </c>
       <c r="K38" s="56"/>
       <c r="L38" s="30">
         <v>5.0000000000000001E-3</v>
@@ -67641,6 +67903,12 @@
       <c r="G39">
         <v>24075311</v>
       </c>
+      <c r="H39" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I39" t="s">
+        <v>1442</v>
+      </c>
       <c r="K39" s="56"/>
       <c r="L39" s="30">
         <v>8.9999999999999993E-3</v>
@@ -67773,6 +68041,12 @@
       <c r="G40" s="52">
         <v>24075675</v>
       </c>
+      <c r="H40" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I40" t="s">
+        <v>1442</v>
+      </c>
       <c r="K40" s="56"/>
       <c r="L40" s="30">
         <v>1E-3</v>
@@ -67905,6 +68179,12 @@
       <c r="G41">
         <v>11846175</v>
       </c>
+      <c r="H41" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I41" t="s">
+        <v>1442</v>
+      </c>
       <c r="K41" s="56"/>
       <c r="L41" s="30">
         <v>3.0000000000000001E-3</v>
@@ -68037,6 +68317,12 @@
       <c r="G42">
         <v>23414009</v>
       </c>
+      <c r="H42" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1442</v>
+      </c>
       <c r="K42" s="56"/>
       <c r="L42" s="30">
         <v>2E-3</v>
@@ -68169,6 +68455,12 @@
       <c r="G43">
         <v>23894328</v>
       </c>
+      <c r="H43" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I43" t="s">
+        <v>1444</v>
+      </c>
       <c r="K43" s="56"/>
       <c r="L43" s="30">
         <v>1E-3</v>
@@ -68301,6 +68593,12 @@
       <c r="G44">
         <v>23896078</v>
       </c>
+      <c r="H44" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I44" t="s">
+        <v>1444</v>
+      </c>
       <c r="K44" s="56"/>
       <c r="L44" s="30">
         <v>2E-3</v>
@@ -68433,6 +68731,12 @@
       <c r="G45">
         <v>23915551</v>
       </c>
+      <c r="H45" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I45" t="s">
+        <v>1446</v>
+      </c>
       <c r="K45" s="56"/>
       <c r="L45" s="30">
         <v>3.0000000000000001E-3</v>
@@ -68565,6 +68869,12 @@
       <c r="G46" s="52">
         <v>22226410</v>
       </c>
+      <c r="H46" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I46" t="s">
+        <v>1444</v>
+      </c>
       <c r="K46" s="56"/>
       <c r="L46" s="30">
         <v>4.0000000000000001E-3</v>
@@ -68697,6 +69007,12 @@
       <c r="G47">
         <v>22226522</v>
       </c>
+      <c r="H47" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I47" t="s">
+        <v>1444</v>
+      </c>
       <c r="K47" s="56"/>
       <c r="L47" s="30">
         <v>3.0000000000000001E-3</v>
@@ -68829,6 +69145,12 @@
       <c r="G48">
         <v>23894328</v>
       </c>
+      <c r="H48" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I48" t="s">
+        <v>1444</v>
+      </c>
       <c r="K48" s="56"/>
       <c r="L48" s="30">
         <v>2E-3</v>
@@ -68961,6 +69283,12 @@
       <c r="G49">
         <v>23902775</v>
       </c>
+      <c r="H49" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I49" t="s">
+        <v>1444</v>
+      </c>
       <c r="K49" s="56"/>
       <c r="L49" s="30">
         <v>3.0000000000000001E-3</v>
@@ -69093,6 +69421,12 @@
       <c r="G50">
         <v>24233042</v>
       </c>
+      <c r="H50" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I50" t="s">
+        <v>1442</v>
+      </c>
       <c r="K50" s="56"/>
       <c r="L50" s="30">
         <v>1.9E-2</v>
@@ -69225,6 +69559,12 @@
       <c r="G51">
         <v>23640374</v>
       </c>
+      <c r="H51" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I51" t="s">
+        <v>1444</v>
+      </c>
       <c r="K51" s="56"/>
       <c r="L51" s="30">
         <v>4.0000000000000001E-3</v>
@@ -69357,6 +69697,12 @@
       <c r="G52">
         <v>23443735</v>
       </c>
+      <c r="H52" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I52" t="s">
+        <v>1444</v>
+      </c>
       <c r="K52" s="56"/>
       <c r="L52" s="30">
         <v>3.0000000000000001E-3</v>
@@ -69489,6 +69835,12 @@
       <c r="G53">
         <v>947100116</v>
       </c>
+      <c r="H53" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I53" t="s">
+        <v>1444</v>
+      </c>
       <c r="K53" s="56"/>
       <c r="L53" s="30">
         <v>9.7000000000000003E-2</v>
@@ -69621,6 +69973,12 @@
       <c r="G54">
         <v>23735817</v>
       </c>
+      <c r="H54" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I54" t="s">
+        <v>1444</v>
+      </c>
       <c r="K54" s="56"/>
       <c r="L54" s="30">
         <v>4.0000000000000001E-3</v>
@@ -69753,8 +70111,12 @@
       <c r="G55" s="2">
         <v>23821889</v>
       </c>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
+      <c r="H55" s="2" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>1444</v>
+      </c>
       <c r="J55" s="2"/>
       <c r="K55" s="57"/>
       <c r="L55" s="34">
@@ -69885,6 +70247,12 @@
       <c r="G56">
         <v>23804938</v>
       </c>
+      <c r="H56" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I56" t="s">
+        <v>1446</v>
+      </c>
       <c r="K56" s="56"/>
       <c r="L56" s="30">
         <v>2.1999999999999999E-2</v>
@@ -70008,6 +70376,12 @@
       <c r="G57">
         <v>23737725</v>
       </c>
+      <c r="H57" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I57" t="s">
+        <v>1444</v>
+      </c>
       <c r="K57" s="56"/>
       <c r="L57" s="30">
         <v>3.0000000000000001E-3</v>
@@ -70131,6 +70505,12 @@
       <c r="G58">
         <v>23713960</v>
       </c>
+      <c r="H58" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I58" t="s">
+        <v>1444</v>
+      </c>
       <c r="K58" s="56"/>
       <c r="L58" s="30">
         <v>1.2999999999999999E-2</v>
@@ -70254,6 +70634,12 @@
       <c r="G59">
         <v>23442333</v>
       </c>
+      <c r="H59" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I59" t="s">
+        <v>1444</v>
+      </c>
       <c r="K59" s="56"/>
       <c r="L59" s="30">
         <v>4.0000000000000001E-3</v>
@@ -70377,6 +70763,12 @@
       <c r="G60">
         <v>23442327</v>
       </c>
+      <c r="H60" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I60" t="s">
+        <v>1444</v>
+      </c>
       <c r="K60" s="56"/>
       <c r="L60" s="30">
         <v>1.0999999999999999E-2</v>
@@ -70500,6 +70892,12 @@
       <c r="G61">
         <v>24526786</v>
       </c>
+      <c r="H61" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I61" t="s">
+        <v>1446</v>
+      </c>
       <c r="K61" s="56"/>
       <c r="L61" s="30">
         <v>8.0000000000000002E-3</v>
@@ -70623,6 +71021,12 @@
       <c r="G62">
         <v>23773217</v>
       </c>
+      <c r="H62" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I62" t="s">
+        <v>1444</v>
+      </c>
       <c r="K62" s="56"/>
       <c r="L62" s="30">
         <v>2E-3</v>
@@ -70746,6 +71150,12 @@
       <c r="G63">
         <v>23763423</v>
       </c>
+      <c r="H63" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I63" t="s">
+        <v>1446</v>
+      </c>
       <c r="K63" s="56"/>
       <c r="L63" s="30">
         <v>6.0000000000000001E-3</v>
@@ -70869,6 +71279,12 @@
       <c r="G64">
         <v>24143410</v>
       </c>
+      <c r="H64" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I64" t="s">
+        <v>1442</v>
+      </c>
       <c r="K64" s="56"/>
       <c r="L64" s="30">
         <v>8.9999999999999993E-3</v>
@@ -70992,6 +71408,12 @@
       <c r="G65">
         <v>23824671</v>
       </c>
+      <c r="H65" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I65" t="s">
+        <v>1444</v>
+      </c>
       <c r="K65" s="56"/>
       <c r="L65" s="30">
         <v>2E-3</v>
@@ -71115,6 +71537,12 @@
       <c r="G66">
         <v>24208825</v>
       </c>
+      <c r="H66" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I66" t="s">
+        <v>1444</v>
+      </c>
       <c r="K66" s="56"/>
       <c r="L66" s="30">
         <v>3.0000000000000001E-3</v>
@@ -71238,6 +71666,12 @@
       <c r="G67">
         <v>23875969</v>
       </c>
+      <c r="H67" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I67" t="s">
+        <v>1446</v>
+      </c>
       <c r="K67" s="56"/>
       <c r="L67" s="30">
         <v>0</v>
@@ -71361,6 +71795,12 @@
       <c r="G68">
         <v>23780817</v>
       </c>
+      <c r="H68" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I68" t="s">
+        <v>1444</v>
+      </c>
       <c r="K68" s="56"/>
       <c r="L68" s="30">
         <v>5.0000000000000001E-3</v>
@@ -71484,6 +71924,12 @@
       <c r="G69">
         <v>23737725</v>
       </c>
+      <c r="H69" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I69" t="s">
+        <v>1444</v>
+      </c>
       <c r="K69" s="56"/>
       <c r="L69" s="30">
         <v>3.0000000000000001E-3</v>
@@ -71607,6 +72053,12 @@
       <c r="G70">
         <v>23760158</v>
       </c>
+      <c r="H70" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I70" t="s">
+        <v>1444</v>
+      </c>
       <c r="K70" s="56"/>
       <c r="L70" s="30">
         <v>1E-3</v>
@@ -71730,6 +72182,12 @@
       <c r="G71">
         <v>23902775</v>
       </c>
+      <c r="H71" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I71" t="s">
+        <v>1444</v>
+      </c>
       <c r="K71" s="56"/>
       <c r="L71" s="30">
         <v>3.0000000000000001E-3</v>
@@ -71853,6 +72311,12 @@
       <c r="G72">
         <v>23753122</v>
       </c>
+      <c r="H72" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I72" t="s">
+        <v>1444</v>
+      </c>
       <c r="K72" s="56"/>
       <c r="L72" s="30">
         <v>0</v>
@@ -71976,6 +72440,12 @@
       <c r="G73">
         <v>23804938</v>
       </c>
+      <c r="H73" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I73" t="s">
+        <v>1446</v>
+      </c>
       <c r="K73" s="56"/>
       <c r="L73" s="30">
         <v>1.9E-2</v>
@@ -72099,6 +72569,12 @@
       <c r="G74">
         <v>23735817</v>
       </c>
+      <c r="H74" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I74" t="s">
+        <v>1444</v>
+      </c>
       <c r="K74" s="56"/>
       <c r="L74" s="30">
         <v>1E-3</v>
@@ -72222,6 +72698,12 @@
       <c r="G75">
         <v>23804876</v>
       </c>
+      <c r="H75" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I75" t="s">
+        <v>1446</v>
+      </c>
       <c r="K75" s="56"/>
       <c r="L75" s="30">
         <v>3.7999999999999999E-2</v>
@@ -72341,6 +72823,12 @@
       </c>
       <c r="G76" s="52">
         <v>23763371</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>1446</v>
       </c>
       <c r="K76" s="56"/>
       <c r="L76" s="53">
@@ -72464,6 +72952,12 @@
       <c r="G77">
         <v>23751918</v>
       </c>
+      <c r="H77" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I77" t="s">
+        <v>1444</v>
+      </c>
       <c r="K77" s="56"/>
       <c r="L77" s="30">
         <v>7.0000000000000001E-3</v>
@@ -72584,6 +73078,12 @@
       <c r="G78">
         <v>23759230</v>
       </c>
+      <c r="H78" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I78" t="s">
+        <v>1446</v>
+      </c>
       <c r="K78" s="56"/>
       <c r="L78" s="30">
         <v>1.2999999999999999E-2</v>
@@ -72707,6 +73207,12 @@
       <c r="G79">
         <v>24075311</v>
       </c>
+      <c r="H79" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I79" t="s">
+        <v>1442</v>
+      </c>
       <c r="K79" s="56"/>
       <c r="L79" s="30">
         <v>8.9999999999999993E-3</v>
@@ -72830,6 +73336,12 @@
       <c r="G80">
         <v>24013535</v>
       </c>
+      <c r="H80" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I80" t="s">
+        <v>1442</v>
+      </c>
       <c r="K80" s="56"/>
       <c r="L80" s="30">
         <v>1.0999999999999999E-2</v>
@@ -72950,6 +73462,12 @@
       <c r="G81">
         <v>23872065</v>
       </c>
+      <c r="H81" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I81" t="s">
+        <v>1446</v>
+      </c>
       <c r="K81" s="56"/>
       <c r="L81" s="30">
         <v>1.9E-2</v>
@@ -73070,6 +73588,12 @@
       <c r="G82">
         <v>23875681</v>
       </c>
+      <c r="H82" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I82" t="s">
+        <v>1446</v>
+      </c>
       <c r="K82" s="56"/>
       <c r="L82" s="30">
         <v>0.01</v>
@@ -73193,6 +73717,12 @@
       <c r="G83">
         <v>23893976</v>
       </c>
+      <c r="H83" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I83" t="s">
+        <v>1444</v>
+      </c>
       <c r="K83" s="56"/>
       <c r="L83" s="30">
         <v>8.9999999999999993E-3</v>
@@ -73316,6 +73846,12 @@
       <c r="G84">
         <v>947100116</v>
       </c>
+      <c r="H84" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I84" t="s">
+        <v>1444</v>
+      </c>
       <c r="K84" s="56"/>
       <c r="L84" s="30">
         <v>0.13700000000000001</v>
@@ -73436,6 +73972,12 @@
       <c r="G85">
         <v>23920620</v>
       </c>
+      <c r="H85" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I85" t="s">
+        <v>1446</v>
+      </c>
       <c r="K85" s="56"/>
       <c r="L85" s="30">
         <v>6.0000000000000001E-3</v>
@@ -73555,6 +74097,12 @@
       </c>
       <c r="G86" s="52">
         <v>23920580</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>1446</v>
       </c>
       <c r="K86" s="56"/>
       <c r="L86" s="53">
@@ -73678,6 +74226,12 @@
       <c r="G87">
         <v>23670969</v>
       </c>
+      <c r="H87" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I87" t="s">
+        <v>1444</v>
+      </c>
       <c r="K87" s="56"/>
       <c r="L87" s="30">
         <v>0.01</v>
@@ -73798,6 +74352,12 @@
       <c r="G88">
         <v>23413599</v>
       </c>
+      <c r="H88" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I88" t="s">
+        <v>1444</v>
+      </c>
       <c r="K88" s="56"/>
       <c r="L88" s="30">
         <v>1.2999999999999999E-2</v>
@@ -73918,6 +74478,12 @@
       <c r="G89">
         <v>23413133</v>
       </c>
+      <c r="H89" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I89" t="s">
+        <v>1444</v>
+      </c>
       <c r="K89" s="56"/>
       <c r="L89" s="30">
         <v>1.0999999999999999E-2</v>
@@ -74041,6 +74607,12 @@
       <c r="G90">
         <v>23821773</v>
       </c>
+      <c r="H90" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I90" t="s">
+        <v>1444</v>
+      </c>
       <c r="K90" s="56"/>
       <c r="L90" s="30">
         <v>7.0000000000000001E-3</v>
@@ -74164,6 +74736,12 @@
       <c r="G91">
         <v>23686254</v>
       </c>
+      <c r="H91" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I91" t="s">
+        <v>1444</v>
+      </c>
       <c r="K91" s="56"/>
       <c r="L91" s="30">
         <v>8.0000000000000002E-3</v>
@@ -74284,6 +74862,12 @@
       <c r="G92">
         <v>23436991</v>
       </c>
+      <c r="H92" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I92" t="s">
+        <v>1444</v>
+      </c>
       <c r="K92" s="56"/>
       <c r="L92" s="30">
         <v>7.0000000000000001E-3</v>
@@ -74404,6 +74988,12 @@
       <c r="G93">
         <v>23437043</v>
       </c>
+      <c r="H93" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I93" t="s">
+        <v>1444</v>
+      </c>
       <c r="K93" s="56"/>
       <c r="L93" s="30">
         <v>4.0000000000000001E-3</v>
@@ -74524,6 +75114,12 @@
       <c r="G94">
         <v>23442233</v>
       </c>
+      <c r="H94" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I94" t="s">
+        <v>1444</v>
+      </c>
       <c r="K94" s="56"/>
       <c r="L94" s="30">
         <v>0.01</v>
@@ -74644,6 +75240,12 @@
       <c r="G95">
         <v>23752476</v>
       </c>
+      <c r="H95" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I95" t="s">
+        <v>1444</v>
+      </c>
       <c r="K95" s="56"/>
       <c r="L95" s="30">
         <v>4.0000000000000001E-3</v>
@@ -74767,6 +75369,12 @@
       <c r="G96">
         <v>23685656</v>
       </c>
+      <c r="H96" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I96" t="s">
+        <v>1442</v>
+      </c>
       <c r="K96" s="56"/>
       <c r="L96" s="30">
         <v>1.7000000000000001E-2</v>
@@ -74890,6 +75498,12 @@
       <c r="G97">
         <v>23889554</v>
       </c>
+      <c r="H97" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I97" t="s">
+        <v>1446</v>
+      </c>
       <c r="K97" s="56"/>
       <c r="L97" s="30">
         <v>1.2999999999999999E-2</v>
@@ -75013,6 +75627,12 @@
       <c r="G98">
         <v>23886302</v>
       </c>
+      <c r="H98" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I98" t="s">
+        <v>1446</v>
+      </c>
       <c r="K98" s="56"/>
       <c r="L98" s="30">
         <v>3.5000000000000003E-2</v>
@@ -75136,6 +75756,12 @@
       <c r="G99">
         <v>24233042</v>
       </c>
+      <c r="H99" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I99" t="s">
+        <v>1442</v>
+      </c>
       <c r="K99" s="56"/>
       <c r="L99" s="30">
         <v>4.0000000000000001E-3</v>
@@ -75259,6 +75885,12 @@
       <c r="G100">
         <v>23443735</v>
       </c>
+      <c r="H100" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I100" t="s">
+        <v>1444</v>
+      </c>
       <c r="K100" s="56"/>
       <c r="L100" s="30">
         <v>1E-3</v>
@@ -75382,6 +76014,12 @@
       <c r="G101">
         <v>23915551</v>
       </c>
+      <c r="H101" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I101" t="s">
+        <v>1446</v>
+      </c>
       <c r="K101" s="56"/>
       <c r="L101" s="30">
         <v>7.0000000000000001E-3</v>
@@ -75505,6 +76143,12 @@
       <c r="G102">
         <v>23894328</v>
       </c>
+      <c r="H102" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I102" t="s">
+        <v>1444</v>
+      </c>
       <c r="K102" s="56"/>
       <c r="L102" s="30">
         <v>0.01</v>
@@ -75628,6 +76272,12 @@
       <c r="G103">
         <v>23902339</v>
       </c>
+      <c r="H103" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I103" t="s">
+        <v>1444</v>
+      </c>
       <c r="K103" s="56"/>
       <c r="L103" s="30">
         <v>1.2999999999999999E-2</v>
@@ -75751,6 +76401,12 @@
       <c r="G104">
         <v>23772775</v>
       </c>
+      <c r="H104" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I104" t="s">
+        <v>1446</v>
+      </c>
       <c r="K104" s="56"/>
       <c r="L104" s="30">
         <v>8.0000000000000002E-3</v>
@@ -75874,6 +76530,12 @@
       <c r="G105">
         <v>23785691</v>
       </c>
+      <c r="H105" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I105" t="s">
+        <v>1446</v>
+      </c>
       <c r="K105" s="56"/>
       <c r="L105" s="30">
         <v>8.0000000000000002E-3</v>
@@ -75997,6 +76659,12 @@
       <c r="G106">
         <v>23894328</v>
       </c>
+      <c r="H106" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I106" t="s">
+        <v>1444</v>
+      </c>
       <c r="K106" s="56"/>
       <c r="L106" s="30">
         <v>6.0000000000000001E-3</v>
@@ -76120,6 +76788,12 @@
       <c r="G107">
         <v>23774363</v>
       </c>
+      <c r="H107" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I107" t="s">
+        <v>1444</v>
+      </c>
       <c r="K107" s="56"/>
       <c r="L107" s="30">
         <v>8.0000000000000002E-3</v>
@@ -76243,6 +76917,12 @@
       <c r="G108">
         <v>24526644</v>
       </c>
+      <c r="H108" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I108" t="s">
+        <v>1446</v>
+      </c>
       <c r="K108" s="56"/>
       <c r="L108" s="30">
         <v>1.2E-2</v>
@@ -76366,6 +77046,12 @@
       <c r="G109">
         <v>23914479</v>
       </c>
+      <c r="H109" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I109" t="s">
+        <v>1446</v>
+      </c>
       <c r="K109" s="56"/>
       <c r="L109" s="30">
         <v>8.0000000000000002E-3</v>
@@ -76489,6 +77175,12 @@
       <c r="G110">
         <v>23940179</v>
       </c>
+      <c r="H110" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I110" t="s">
+        <v>1446</v>
+      </c>
       <c r="K110" s="56"/>
       <c r="L110" s="30">
         <v>1.2E-2</v>
@@ -76612,6 +77304,12 @@
       <c r="G111">
         <v>23785691</v>
       </c>
+      <c r="H111" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I111" t="s">
+        <v>1446</v>
+      </c>
       <c r="K111" s="56"/>
       <c r="L111" s="30">
         <v>0.01</v>
@@ -76735,6 +77433,12 @@
       <c r="G112">
         <v>23706304</v>
       </c>
+      <c r="H112" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I112" t="s">
+        <v>1444</v>
+      </c>
       <c r="K112" s="56"/>
       <c r="L112" s="30">
         <v>1.0999999999999999E-2</v>
@@ -76858,6 +77562,12 @@
       <c r="G113">
         <v>947070128</v>
       </c>
+      <c r="H113" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I113" t="s">
+        <v>1442</v>
+      </c>
       <c r="K113" s="56"/>
       <c r="L113" s="30">
         <v>1.6E-2</v>
@@ -76981,6 +77691,12 @@
       <c r="G114">
         <v>23945915</v>
       </c>
+      <c r="H114" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I114" t="s">
+        <v>1444</v>
+      </c>
       <c r="K114" s="56"/>
       <c r="L114" s="30">
         <v>8.0000000000000002E-3</v>
@@ -77104,6 +77820,12 @@
       <c r="G115" s="52">
         <v>22226410</v>
       </c>
+      <c r="H115" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I115" t="s">
+        <v>1444</v>
+      </c>
       <c r="K115" s="56"/>
       <c r="L115" s="30">
         <v>4.0000000000000001E-3</v>
@@ -77227,6 +77949,12 @@
       <c r="G116">
         <v>23872825</v>
       </c>
+      <c r="H116" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I116" t="s">
+        <v>1446</v>
+      </c>
       <c r="K116" s="56"/>
       <c r="L116" s="30">
         <v>8.0000000000000002E-3</v>
@@ -77350,6 +78078,12 @@
       <c r="G117">
         <v>24084416</v>
       </c>
+      <c r="H117" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I117" t="s">
+        <v>1444</v>
+      </c>
       <c r="K117" s="56"/>
       <c r="L117" s="30">
         <v>6.0000000000000001E-3</v>
@@ -77473,6 +78207,12 @@
       <c r="G118">
         <v>24084412</v>
       </c>
+      <c r="H118" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I118" t="s">
+        <v>1444</v>
+      </c>
       <c r="K118" s="56"/>
       <c r="L118" s="30">
         <v>6.0000000000000001E-3</v>
@@ -77596,6 +78336,12 @@
       <c r="G119">
         <v>23700493</v>
       </c>
+      <c r="H119" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I119" t="s">
+        <v>1444</v>
+      </c>
       <c r="K119" s="56"/>
       <c r="L119" s="30">
         <v>0.17699999999999999</v>
@@ -77719,6 +78465,12 @@
       <c r="G120">
         <v>23428648</v>
       </c>
+      <c r="H120" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I120" t="s">
+        <v>1444</v>
+      </c>
       <c r="K120" s="56"/>
       <c r="L120" s="30">
         <v>7.0000000000000001E-3</v>
@@ -77842,6 +78594,12 @@
       <c r="G121">
         <v>23671143</v>
       </c>
+      <c r="H121" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I121" t="s">
+        <v>1444</v>
+      </c>
       <c r="K121" s="56"/>
       <c r="L121" s="30">
         <v>7.0000000000000001E-3</v>
@@ -77965,6 +78723,12 @@
       <c r="G122">
         <v>23671695</v>
       </c>
+      <c r="H122" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I122" t="s">
+        <v>1444</v>
+      </c>
       <c r="K122" s="56"/>
       <c r="L122" s="30">
         <v>5.0000000000000001E-3</v>
@@ -78088,6 +78852,12 @@
       <c r="G123">
         <v>23686016</v>
       </c>
+      <c r="H123" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I123" t="s">
+        <v>1444</v>
+      </c>
       <c r="K123" s="56"/>
       <c r="L123" s="30">
         <v>8.9999999999999993E-3</v>
@@ -78211,6 +78981,12 @@
       <c r="G124">
         <v>23719073</v>
       </c>
+      <c r="H124" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I124" t="s">
+        <v>1442</v>
+      </c>
       <c r="K124" s="56"/>
       <c r="L124" s="30">
         <v>1.4E-2</v>
@@ -78333,6 +79109,12 @@
       </c>
       <c r="G125" s="2">
         <v>24219761</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I125" s="2" t="s">
+        <v>1444</v>
       </c>
       <c r="K125" s="57"/>
       <c r="L125" s="34">
@@ -78462,6 +79244,12 @@
       <c r="G126">
         <v>24528218</v>
       </c>
+      <c r="H126" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I126" t="s">
+        <v>1446</v>
+      </c>
       <c r="K126" s="56"/>
       <c r="L126" s="30">
         <v>5.5E-2</v>
@@ -78588,6 +79376,12 @@
       <c r="G127">
         <v>23659640</v>
       </c>
+      <c r="H127" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I127" t="s">
+        <v>1442</v>
+      </c>
       <c r="K127" s="56"/>
       <c r="L127" s="30">
         <v>5.5E-2</v>
@@ -78714,6 +79508,12 @@
       <c r="G128">
         <v>23824881</v>
       </c>
+      <c r="H128" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I128" t="s">
+        <v>1444</v>
+      </c>
       <c r="K128" s="56"/>
       <c r="L128" s="30">
         <v>0.01</v>
@@ -78840,6 +79640,12 @@
       <c r="G129">
         <v>24207875</v>
       </c>
+      <c r="H129" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I129" t="s">
+        <v>1444</v>
+      </c>
       <c r="K129" s="56"/>
       <c r="L129" s="30">
         <v>8.0000000000000002E-3</v>
@@ -78966,6 +79772,12 @@
       <c r="G130">
         <v>23889622</v>
       </c>
+      <c r="H130" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I130" t="s">
+        <v>1446</v>
+      </c>
       <c r="K130" s="56"/>
       <c r="L130" s="30">
         <v>1.7000000000000001E-2</v>
@@ -79092,6 +79904,12 @@
       <c r="G131">
         <v>24224945</v>
       </c>
+      <c r="H131" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I131" t="s">
+        <v>1444</v>
+      </c>
       <c r="K131" s="56"/>
       <c r="L131" s="30">
         <v>1E-3</v>
@@ -79218,6 +80036,12 @@
       <c r="G132">
         <v>23876833</v>
       </c>
+      <c r="H132" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I132" t="s">
+        <v>1446</v>
+      </c>
       <c r="K132" s="56"/>
       <c r="L132" s="30">
         <v>8.9999999999999993E-3</v>
@@ -79344,6 +80168,12 @@
       <c r="G133">
         <v>23894328</v>
       </c>
+      <c r="H133" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I133" t="s">
+        <v>1444</v>
+      </c>
       <c r="K133" s="56"/>
       <c r="L133" s="30">
         <v>7.0000000000000001E-3</v>
@@ -79470,6 +80300,12 @@
       <c r="G134">
         <v>947100116</v>
       </c>
+      <c r="H134" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I134" t="s">
+        <v>1444</v>
+      </c>
       <c r="K134" s="56"/>
       <c r="L134" s="30">
         <v>7.4999999999999997E-2</v>
@@ -79596,6 +80432,12 @@
       <c r="G135">
         <v>23785691</v>
       </c>
+      <c r="H135" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I135" t="s">
+        <v>1446</v>
+      </c>
       <c r="K135" s="56"/>
       <c r="L135" s="30">
         <v>8.0000000000000002E-3</v>
@@ -79722,6 +80564,12 @@
       <c r="G136">
         <v>23785691</v>
       </c>
+      <c r="H136" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I136" t="s">
+        <v>1446</v>
+      </c>
       <c r="K136" s="56"/>
       <c r="L136" s="30">
         <v>5.0000000000000001E-3</v>
@@ -79848,6 +80696,12 @@
       <c r="G137">
         <v>23886302</v>
       </c>
+      <c r="H137" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I137" t="s">
+        <v>1446</v>
+      </c>
       <c r="K137" s="56"/>
       <c r="L137" s="30">
         <v>1.6E-2</v>
@@ -79974,6 +80828,12 @@
       <c r="G138">
         <v>23893976</v>
       </c>
+      <c r="H138" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I138" t="s">
+        <v>1444</v>
+      </c>
       <c r="K138" s="56"/>
       <c r="L138" s="30">
         <v>7.0000000000000001E-3</v>
@@ -80100,6 +80960,12 @@
       <c r="G139">
         <v>23763423</v>
       </c>
+      <c r="H139" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I139" t="s">
+        <v>1446</v>
+      </c>
       <c r="K139" s="56"/>
       <c r="L139" s="30">
         <v>1.2999999999999999E-2</v>
@@ -80226,6 +81092,12 @@
       <c r="G140">
         <v>23880848</v>
       </c>
+      <c r="H140" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I140" t="s">
+        <v>1446</v>
+      </c>
       <c r="K140" s="56"/>
       <c r="L140" s="30">
         <v>1.6E-2</v>
@@ -80352,6 +81224,12 @@
       <c r="G141">
         <v>23760158</v>
       </c>
+      <c r="H141" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I141" t="s">
+        <v>1444</v>
+      </c>
       <c r="K141" s="56"/>
       <c r="L141" s="30">
         <v>7.0000000000000001E-3</v>
@@ -80478,6 +81356,12 @@
       <c r="G142">
         <v>23780491</v>
       </c>
+      <c r="H142" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I142" t="s">
+        <v>1446</v>
+      </c>
       <c r="K142" s="56"/>
       <c r="L142" s="30">
         <v>5.0000000000000001E-3</v>
@@ -80604,6 +81488,12 @@
       <c r="G143" s="52">
         <v>22226410</v>
       </c>
+      <c r="H143" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I143" t="s">
+        <v>1444</v>
+      </c>
       <c r="K143" s="56"/>
       <c r="L143" s="30">
         <v>6.0000000000000001E-3</v>
@@ -80730,6 +81620,12 @@
       <c r="G144">
         <v>23902339</v>
       </c>
+      <c r="H144" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I144" t="s">
+        <v>1444</v>
+      </c>
       <c r="K144" s="56"/>
       <c r="L144" s="30">
         <v>7.0000000000000001E-3</v>
@@ -80856,6 +81752,12 @@
       <c r="G145">
         <v>23671143</v>
       </c>
+      <c r="H145" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I145" t="s">
+        <v>1444</v>
+      </c>
       <c r="K145" s="56"/>
       <c r="L145" s="30">
         <v>0</v>
@@ -80982,6 +81884,12 @@
       <c r="G146">
         <v>23763329</v>
       </c>
+      <c r="H146" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I146" t="s">
+        <v>1446</v>
+      </c>
       <c r="K146" s="56"/>
       <c r="L146" s="30">
         <v>1.9E-2</v>
@@ -81108,6 +82016,12 @@
       <c r="G147">
         <v>24208825</v>
       </c>
+      <c r="H147" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I147" t="s">
+        <v>1444</v>
+      </c>
       <c r="K147" s="56"/>
       <c r="L147" s="30">
         <v>0</v>
@@ -81234,6 +82148,12 @@
       <c r="G148">
         <v>23940179</v>
       </c>
+      <c r="H148" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I148" t="s">
+        <v>1446</v>
+      </c>
       <c r="K148" s="56"/>
       <c r="L148" s="30">
         <v>1.4E-2</v>
@@ -81360,6 +82280,12 @@
       <c r="G149">
         <v>23772873</v>
       </c>
+      <c r="H149" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I149" t="s">
+        <v>1444</v>
+      </c>
       <c r="K149" s="56"/>
       <c r="L149" s="30">
         <v>5.0000000000000001E-3</v>
@@ -81486,6 +82412,12 @@
       <c r="G150">
         <v>23772873</v>
       </c>
+      <c r="H150" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I150" t="s">
+        <v>1444</v>
+      </c>
       <c r="K150" s="56"/>
       <c r="L150" s="30">
         <v>4.0000000000000001E-3</v>
@@ -81612,6 +82544,12 @@
       <c r="G151">
         <v>24526820</v>
       </c>
+      <c r="H151" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I151" t="s">
+        <v>1446</v>
+      </c>
       <c r="K151" s="56"/>
       <c r="L151" s="30">
         <v>0.01</v>
@@ -81738,6 +82676,12 @@
       <c r="G152">
         <v>23671695</v>
       </c>
+      <c r="H152" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I152" t="s">
+        <v>1444</v>
+      </c>
       <c r="K152" s="56"/>
       <c r="L152" s="30">
         <v>4.0000000000000001E-3</v>
@@ -81864,6 +82808,12 @@
       <c r="G153">
         <v>23780461</v>
       </c>
+      <c r="H153" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I153" t="s">
+        <v>1446</v>
+      </c>
       <c r="K153" s="56"/>
       <c r="L153" s="30">
         <v>6.0000000000000001E-3</v>
@@ -81990,6 +82940,12 @@
       <c r="G154">
         <v>23685656</v>
       </c>
+      <c r="H154" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I154" t="s">
+        <v>1442</v>
+      </c>
       <c r="K154" s="56"/>
       <c r="L154" s="30">
         <v>1.0999999999999999E-2</v>
@@ -82116,6 +83072,12 @@
       <c r="G155">
         <v>24143410</v>
       </c>
+      <c r="H155" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I155" t="s">
+        <v>1442</v>
+      </c>
       <c r="K155" s="56"/>
       <c r="L155" s="30">
         <v>8.9999999999999993E-3</v>
@@ -82242,6 +83204,12 @@
       <c r="G156">
         <v>23685514</v>
       </c>
+      <c r="H156" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I156" t="s">
+        <v>1442</v>
+      </c>
       <c r="K156" s="56"/>
       <c r="L156" s="30">
         <v>4.0000000000000001E-3</v>
@@ -82368,6 +83336,12 @@
       <c r="G157">
         <v>24541699</v>
       </c>
+      <c r="H157" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I157" t="s">
+        <v>1442</v>
+      </c>
       <c r="K157" s="56"/>
       <c r="L157" s="30">
         <v>1.7000000000000001E-2</v>
@@ -82494,6 +83468,12 @@
       <c r="G158">
         <v>24541701</v>
       </c>
+      <c r="H158" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I158" t="s">
+        <v>1442</v>
+      </c>
       <c r="K158" s="56"/>
       <c r="L158" s="30">
         <v>1.9E-2</v>
@@ -82620,6 +83600,12 @@
       <c r="G159">
         <v>23773217</v>
       </c>
+      <c r="H159" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I159" t="s">
+        <v>1444</v>
+      </c>
       <c r="K159" s="56"/>
       <c r="L159" s="30">
         <v>0</v>
@@ -82746,6 +83732,12 @@
       <c r="G160">
         <v>23949615</v>
       </c>
+      <c r="H160" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I160" t="s">
+        <v>1446</v>
+      </c>
       <c r="K160" s="56"/>
       <c r="L160" s="30">
         <v>6.0000000000000001E-3</v>
@@ -82872,6 +83864,12 @@
       <c r="G161">
         <v>23700833</v>
       </c>
+      <c r="H161" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I161" t="s">
+        <v>1444</v>
+      </c>
       <c r="K161" s="56"/>
       <c r="L161" s="30">
         <v>1.0999999999999999E-2</v>
@@ -82998,6 +83996,12 @@
       <c r="G162">
         <v>23718751</v>
       </c>
+      <c r="H162" t="s">
+        <v>1441</v>
+      </c>
+      <c r="I162" t="s">
+        <v>1442</v>
+      </c>
       <c r="K162" s="56"/>
       <c r="L162" s="30">
         <v>1.2E-2</v>
@@ -83124,6 +84128,12 @@
       <c r="G163">
         <v>23894288</v>
       </c>
+      <c r="H163" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I163" t="s">
+        <v>1444</v>
+      </c>
       <c r="K163" s="56"/>
       <c r="L163" s="30">
         <v>1E-3</v>
@@ -83250,6 +84260,12 @@
       <c r="G164">
         <v>23889554</v>
       </c>
+      <c r="H164" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I164" t="s">
+        <v>1446</v>
+      </c>
       <c r="K164" s="56"/>
       <c r="L164" s="30">
         <v>6.0000000000000001E-3</v>
@@ -83376,6 +84392,12 @@
       <c r="G165">
         <v>24026308</v>
       </c>
+      <c r="H165" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I165" t="s">
+        <v>1444</v>
+      </c>
       <c r="K165" s="56"/>
       <c r="L165" s="30">
         <v>3.0000000000000001E-3</v>
@@ -83502,6 +84524,12 @@
       <c r="G166">
         <v>23735817</v>
       </c>
+      <c r="H166" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I166" t="s">
+        <v>1444</v>
+      </c>
       <c r="K166" s="56"/>
       <c r="L166" s="30">
         <v>5.0000000000000001E-3</v>
@@ -83628,6 +84656,12 @@
       <c r="G167">
         <v>23737725</v>
       </c>
+      <c r="H167" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I167" t="s">
+        <v>1444</v>
+      </c>
       <c r="K167" s="56"/>
       <c r="L167" s="30">
         <v>8.9999999999999993E-3</v>
@@ -83754,6 +84788,12 @@
       <c r="G168">
         <v>23737725</v>
       </c>
+      <c r="H168" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I168" t="s">
+        <v>1444</v>
+      </c>
       <c r="K168" s="56"/>
       <c r="L168" s="30">
         <v>8.9999999999999993E-3</v>
@@ -83880,6 +84920,12 @@
       <c r="G169">
         <v>24219761</v>
       </c>
+      <c r="H169" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I169" t="s">
+        <v>1444</v>
+      </c>
       <c r="K169" s="56"/>
       <c r="L169" s="30">
         <v>7.0000000000000001E-3</v>
@@ -84006,6 +85052,12 @@
       <c r="G170">
         <v>23713960</v>
       </c>
+      <c r="H170" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I170" t="s">
+        <v>1444</v>
+      </c>
       <c r="K170" s="56"/>
       <c r="L170" s="30">
         <v>8.9999999999999993E-3</v>
@@ -84132,6 +85184,12 @@
       <c r="G171">
         <v>23804938</v>
       </c>
+      <c r="H171" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I171" t="s">
+        <v>1446</v>
+      </c>
       <c r="K171" s="56"/>
       <c r="L171" s="30">
         <v>2.1000000000000001E-2</v>
@@ -84258,6 +85316,12 @@
       <c r="G172">
         <v>23804938</v>
       </c>
+      <c r="H172" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I172" t="s">
+        <v>1446</v>
+      </c>
       <c r="K172" s="56"/>
       <c r="L172" s="30">
         <v>2.4E-2</v>
@@ -84384,6 +85448,12 @@
       <c r="G173">
         <v>24084416</v>
       </c>
+      <c r="H173" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I173" t="s">
+        <v>1444</v>
+      </c>
       <c r="K173" s="56"/>
       <c r="L173" s="30">
         <v>8.0000000000000002E-3</v>
@@ -84510,6 +85580,12 @@
       <c r="G174">
         <v>24223737</v>
       </c>
+      <c r="H174" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I174" t="s">
+        <v>1444</v>
+      </c>
       <c r="K174" s="56"/>
       <c r="L174" s="30">
         <v>1E-3</v>
@@ -84636,6 +85712,12 @@
       <c r="G175">
         <v>24084324</v>
       </c>
+      <c r="H175" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I175" t="s">
+        <v>1444</v>
+      </c>
       <c r="K175" s="56"/>
       <c r="L175" s="30">
         <v>7.0000000000000001E-3</v>
@@ -84762,6 +85844,12 @@
       <c r="G176">
         <v>23815284</v>
       </c>
+      <c r="H176" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I176" t="s">
+        <v>1446</v>
+      </c>
       <c r="K176" s="56"/>
       <c r="L176" s="30">
         <v>0</v>
@@ -84888,6 +85976,12 @@
       <c r="G177">
         <v>23824671</v>
       </c>
+      <c r="H177" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I177" t="s">
+        <v>1444</v>
+      </c>
       <c r="K177" s="56"/>
       <c r="L177" s="30">
         <v>0</v>
@@ -85014,6 +86108,12 @@
       <c r="G178">
         <v>23681167</v>
       </c>
+      <c r="H178" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I178" t="s">
+        <v>1444</v>
+      </c>
       <c r="K178" s="56"/>
       <c r="L178" s="30">
         <v>1.4999999999999999E-2</v>
@@ -85140,6 +86240,12 @@
       <c r="G179">
         <v>24219829</v>
       </c>
+      <c r="H179" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I179" t="s">
+        <v>1444</v>
+      </c>
       <c r="K179" s="56"/>
       <c r="L179" s="30">
         <v>6.0000000000000001E-3</v>
@@ -85266,6 +86372,12 @@
       <c r="G180">
         <v>24013535</v>
       </c>
+      <c r="H180" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I180" t="s">
+        <v>1442</v>
+      </c>
       <c r="K180" s="56"/>
       <c r="L180" s="30">
         <v>1.7000000000000001E-2</v>
@@ -85392,6 +86504,12 @@
       <c r="G181">
         <v>23915551</v>
       </c>
+      <c r="H181" t="s">
+        <v>1445</v>
+      </c>
+      <c r="I181" t="s">
+        <v>1446</v>
+      </c>
       <c r="K181" s="56"/>
       <c r="L181" s="30">
         <v>4.0000000000000001E-3</v>
@@ -85518,6 +86636,12 @@
       <c r="G182">
         <v>23815040</v>
       </c>
+      <c r="H182" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I182" t="s">
+        <v>1446</v>
+      </c>
       <c r="K182" s="56"/>
       <c r="L182" s="30">
         <v>5.8999999999999997E-2</v>
@@ -85644,6 +86768,12 @@
       <c r="G183">
         <v>23700493</v>
       </c>
+      <c r="H183" t="s">
+        <v>1449</v>
+      </c>
+      <c r="I183" t="s">
+        <v>1444</v>
+      </c>
       <c r="K183" s="56"/>
       <c r="L183" s="30">
         <v>2.4E-2</v>
@@ -85769,6 +86899,12 @@
       </c>
       <c r="G184" s="2">
         <v>23442287</v>
+      </c>
+      <c r="H184" s="2" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I184" s="2" t="s">
+        <v>1444</v>
       </c>
       <c r="K184" s="57"/>
       <c r="L184" s="34">

</xml_diff>